<commit_message>
feat: new version document
</commit_message>
<xml_diff>
--- a/public/templates/tariff-library-template.xlsx
+++ b/public/templates/tariff-library-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Море" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
   <si>
     <t xml:space="preserve">POL</t>
   </si>
@@ -67,6 +67,12 @@
     <t xml:space="preserve">40HC</t>
   </si>
   <si>
+    <t xml:space="preserve">Пункт назначения (жд)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Станция назначения</t>
+  </si>
+  <si>
     <t xml:space="preserve">ЖД оператор</t>
   </si>
   <si>
@@ -101,6 +107,15 @@
   </si>
   <si>
     <t xml:space="preserve">Автомобильная доставка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Терминальный сбор / Раскредитация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комментарии – Доставка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комментарии - Раскредитация </t>
   </si>
   <si>
     <t xml:space="preserve">20DRY&lt;18т</t>
@@ -205,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,15 +229,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,23 +258,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="8.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="255.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="51.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,41 +351,6 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A1:A3"/>
@@ -405,153 +381,135 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="105.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="51.42"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-    </row>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="O3" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -568,61 +526,61 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1048576"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O41" activeCellId="0" sqref="O41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="9.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="16.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="33.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="9.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="2" width="9.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="16.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="13.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="2" width="9.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="9.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="20.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="3" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="41.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="3" width="9.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="K1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="4"/>
       <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
@@ -632,21 +590,21 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
         <v>9</v>
@@ -661,19 +619,19 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
         <v>12</v>
@@ -685,6 +643,181 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="40.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="36.11"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -759,144 +892,22 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H1048576"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="15">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="M1:M3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>